<commit_message>
Fixed the duplicate designations issue
</commit_message>
<xml_diff>
--- a/src/test/TestData/SkillMater.xlsx
+++ b/src/test/TestData/SkillMater.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piyush.Wadhwa\IdeaProjects\Automation\RMT\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A890185-7367-41AC-9B01-05EAE169ACE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ADAD94-816B-406F-95E7-2340E354FDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1387,7 +1387,7 @@
     <t>Newly Crea+C2+A+A2:P2</t>
   </si>
   <si>
-    <t>PW_2032_21</t>
+    <t>PW_2032_36</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Reduce the sleep time to 0.1 sec
</commit_message>
<xml_diff>
--- a/src/test/TestData/SkillMater.xlsx
+++ b/src/test/TestData/SkillMater.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piyush.Wadhwa\IdeaProjects\Automation\RMT\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ADAD94-816B-406F-95E7-2340E354FDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B7F49C-00E1-4310-A49E-0C344AD9A51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1387,7 +1387,7 @@
     <t>Newly Crea+C2+A+A2:P2</t>
   </si>
   <si>
-    <t>PW_2032_36</t>
+    <t>PW_2032_38</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added test for requsition page and Report generation logic
</commit_message>
<xml_diff>
--- a/src/test/TestData/SkillMater.xlsx
+++ b/src/test/TestData/SkillMater.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piyush.Wadhwa\IdeaProjects\Automation\RMT\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B7F49C-00E1-4310-A49E-0C344AD9A51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755BD5F1-FD87-41CA-8958-F446352A621A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SkillMaster!$C$1:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SkillMaster!$C$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1384,10 +1384,10 @@
     <t>GOA</t>
   </si>
   <si>
-    <t>Newly Crea+C2+A+A2:P2</t>
-  </si>
-  <si>
-    <t>PW_2032_38</t>
+    <t>Newly Crea+C2+A+A2:P796</t>
+  </si>
+  <si>
+    <t>PW_2033_1003</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added retry logic and headless & Incognito logic
</commit_message>
<xml_diff>
--- a/src/test/TestData/SkillMater.xlsx
+++ b/src/test/TestData/SkillMater.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piyush.Wadhwa\IdeaProjects\Automation\RMT\src\test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725431D8-61D8-4917-8FE3-AF65551295D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362BE8CB-7D09-4836-9987-989E4F95C872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1931,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3516,7 +3516,7 @@
       <c r="B23" t="s">
         <v>189</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="6" t="s">
         <v>190</v>
       </c>
       <c r="D23" s="1" t="s">

</xml_diff>